<commit_message>
update before create dev branch
</commit_message>
<xml_diff>
--- a/4. Document/MicroMouse2024_Roadmap.xlsx
+++ b/4. Document/MicroMouse2024_Roadmap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1. Phenikaa University\AML\0. Project\7. MicroMouse_2024\4. Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAF47FB-1B0A-4782-951C-CFDAFA2725D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9D0FF5-D3B9-4AFF-8761-0B709CF677B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11040" yWindow="17172" windowWidth="23256" windowHeight="12456" xr2:uid="{5F5C8CA6-E2DE-437A-803B-FCB446A740AB}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="30912" windowHeight="16752" xr2:uid="{5F5C8CA6-E2DE-437A-803B-FCB446A740AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1043,80 +1043,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1457,44 +1457,44 @@
   <dimension ref="A2:AL137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.33203125" customWidth="1"/>
-    <col min="2" max="2" width="44.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="72.28515625" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="79" t="s">
+    <row r="2" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-    </row>
-    <row r="4" spans="2:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+    </row>
+    <row r="4" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-    </row>
-    <row r="5" spans="2:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+    </row>
+    <row r="5" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
@@ -1506,7 +1506,7 @@
       <c r="J5" s="38"/>
       <c r="K5" s="38"/>
     </row>
-    <row r="6" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D6" s="40" t="s">
         <v>17</v>
       </c>
@@ -1515,7 +1515,7 @@
       <c r="G6" s="40"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D7" s="40" t="s">
         <v>19</v>
       </c>
@@ -1524,14 +1524,14 @@
       <c r="G7" s="40"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D8" s="39"/>
       <c r="E8" s="40"/>
       <c r="F8" s="40"/>
       <c r="G8" s="40"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D9" s="40" t="s">
         <v>10</v>
       </c>
@@ -1540,14 +1540,14 @@
       <c r="G9" s="40"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D10" s="39"/>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
       <c r="G10" s="40"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D11" s="40" t="s">
         <v>11</v>
       </c>
@@ -1556,200 +1556,200 @@
       <c r="G11" s="40"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="2:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D13" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="101" t="s">
+      <c r="E13" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="102"/>
-      <c r="G13" s="103"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="81"/>
       <c r="H13" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="101" t="s">
+      <c r="I13" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="102"/>
-      <c r="K13" s="103"/>
-    </row>
-    <row r="14" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J13" s="80"/>
+      <c r="K13" s="81"/>
+    </row>
+    <row r="14" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D14" s="43">
         <v>1</v>
       </c>
-      <c r="E14" s="95" t="s">
+      <c r="E14" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="96"/>
-      <c r="G14" s="97"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="84"/>
       <c r="H14" s="44">
         <v>1</v>
       </c>
-      <c r="I14" s="95"/>
-      <c r="J14" s="96"/>
-      <c r="K14" s="97"/>
-    </row>
-    <row r="15" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I14" s="82"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="84"/>
+    </row>
+    <row r="15" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D15" s="43">
         <v>2</v>
       </c>
-      <c r="E15" s="95" t="s">
+      <c r="E15" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="96"/>
-      <c r="G15" s="97"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="84"/>
       <c r="H15" s="44">
         <v>1</v>
       </c>
-      <c r="I15" s="95"/>
-      <c r="J15" s="96"/>
-      <c r="K15" s="97"/>
-    </row>
-    <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I15" s="82"/>
+      <c r="J15" s="83"/>
+      <c r="K15" s="84"/>
+    </row>
+    <row r="16" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D16" s="43">
         <v>3</v>
       </c>
-      <c r="E16" s="95" t="s">
+      <c r="E16" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="97"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="84"/>
       <c r="H16" s="45">
         <v>2</v>
       </c>
-      <c r="I16" s="95"/>
-      <c r="J16" s="96"/>
-      <c r="K16" s="97"/>
-    </row>
-    <row r="17" spans="1:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I16" s="82"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="84"/>
+    </row>
+    <row r="17" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="46">
         <v>4</v>
       </c>
-      <c r="E17" s="98" t="s">
+      <c r="E17" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="99"/>
-      <c r="G17" s="100"/>
+      <c r="F17" s="91"/>
+      <c r="G17" s="92"/>
       <c r="H17" s="46">
         <v>2</v>
       </c>
-      <c r="I17" s="98"/>
-      <c r="J17" s="99"/>
-      <c r="K17" s="100"/>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="C20" s="80" t="s">
+      <c r="I17" s="90"/>
+      <c r="J17" s="91"/>
+      <c r="K17" s="92"/>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="C20" s="102" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="80"/>
-      <c r="K20" s="80"/>
-      <c r="L20" s="80"/>
-      <c r="M20" s="80"/>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="80"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="80"/>
-      <c r="K21" s="80"/>
-      <c r="L21" s="80"/>
-      <c r="M21" s="80"/>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A26" s="79" t="s">
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="102"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="102"/>
+      <c r="J20" s="102"/>
+      <c r="K20" s="102"/>
+      <c r="L20" s="102"/>
+      <c r="M20" s="102"/>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="C21" s="102"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="102"/>
+      <c r="I21" s="102"/>
+      <c r="J21" s="102"/>
+      <c r="K21" s="102"/>
+      <c r="L21" s="102"/>
+      <c r="M21" s="102"/>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A26" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="79"/>
-      <c r="C26" s="79"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="79"/>
-      <c r="I26" s="79"/>
-      <c r="J26" s="79"/>
-    </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A27" s="79"/>
-      <c r="B27" s="79"/>
-      <c r="C27" s="79"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="79"/>
-      <c r="J27" s="79"/>
-    </row>
-    <row r="28" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="95"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="95"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="95"/>
+      <c r="I26" s="95"/>
+      <c r="J26" s="95"/>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A27" s="95"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="95"/>
+      <c r="J27" s="95"/>
+    </row>
+    <row r="28" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="81" t="s">
+      <c r="D29" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="82"/>
-      <c r="F29" s="82"/>
-      <c r="G29" s="82"/>
-      <c r="H29" s="82"/>
-      <c r="I29" s="82"/>
-      <c r="J29" s="83"/>
-      <c r="K29" s="92" t="s">
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
+      <c r="H29" s="86"/>
+      <c r="I29" s="86"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="L29" s="93"/>
-      <c r="M29" s="93"/>
-      <c r="N29" s="93"/>
-      <c r="O29" s="93"/>
-      <c r="P29" s="93"/>
-      <c r="Q29" s="93"/>
-      <c r="R29" s="81" t="s">
+      <c r="L29" s="89"/>
+      <c r="M29" s="89"/>
+      <c r="N29" s="89"/>
+      <c r="O29" s="89"/>
+      <c r="P29" s="89"/>
+      <c r="Q29" s="89"/>
+      <c r="R29" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="S29" s="82"/>
-      <c r="T29" s="82"/>
-      <c r="U29" s="82"/>
-      <c r="V29" s="82"/>
-      <c r="W29" s="82"/>
-      <c r="X29" s="83"/>
-      <c r="Y29" s="81" t="s">
+      <c r="S29" s="86"/>
+      <c r="T29" s="86"/>
+      <c r="U29" s="86"/>
+      <c r="V29" s="86"/>
+      <c r="W29" s="86"/>
+      <c r="X29" s="87"/>
+      <c r="Y29" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="Z29" s="84"/>
-      <c r="AA29" s="84"/>
-      <c r="AB29" s="84"/>
-      <c r="AC29" s="84"/>
-      <c r="AD29" s="84"/>
-      <c r="AE29" s="85"/>
-      <c r="AF29" s="81" t="s">
+      <c r="Z29" s="93"/>
+      <c r="AA29" s="93"/>
+      <c r="AB29" s="93"/>
+      <c r="AC29" s="93"/>
+      <c r="AD29" s="93"/>
+      <c r="AE29" s="94"/>
+      <c r="AF29" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="AG29" s="84"/>
-      <c r="AH29" s="84"/>
-      <c r="AI29" s="84"/>
-      <c r="AJ29" s="84"/>
-      <c r="AK29" s="84"/>
-      <c r="AL29" s="85"/>
-    </row>
-    <row r="30" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AG29" s="93"/>
+      <c r="AH29" s="93"/>
+      <c r="AI29" s="93"/>
+      <c r="AJ29" s="93"/>
+      <c r="AK29" s="93"/>
+      <c r="AL29" s="94"/>
+    </row>
+    <row r="30" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>6</v>
       </c>
@@ -1857,7 +1857,7 @@
       <c r="AK30" s="8"/>
       <c r="AL30" s="12"/>
     </row>
-    <row r="31" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>28</v>
       </c>
@@ -1903,7 +1903,7 @@
       <c r="AK31" s="17"/>
       <c r="AL31" s="18"/>
     </row>
-    <row r="32" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>45</v>
       </c>
@@ -1947,7 +1947,7 @@
       <c r="AK32" s="17"/>
       <c r="AL32" s="18"/>
     </row>
-    <row r="33" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>37</v>
       </c>
@@ -1991,7 +1991,7 @@
       <c r="AK33" s="17"/>
       <c r="AL33" s="18"/>
     </row>
-    <row r="34" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>38</v>
       </c>
@@ -2037,7 +2037,7 @@
       <c r="AK34" s="17"/>
       <c r="AL34" s="18"/>
     </row>
-    <row r="35" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>39</v>
       </c>
@@ -2083,7 +2083,7 @@
       <c r="AK35" s="17"/>
       <c r="AL35" s="18"/>
     </row>
-    <row r="36" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>40</v>
       </c>
@@ -2129,7 +2129,7 @@
       <c r="AK36" s="17"/>
       <c r="AL36" s="18"/>
     </row>
-    <row r="37" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>41</v>
       </c>
@@ -2173,7 +2173,7 @@
       <c r="AK37" s="17"/>
       <c r="AL37" s="18"/>
     </row>
-    <row r="38" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>42</v>
       </c>
@@ -2219,7 +2219,7 @@
       <c r="AK38" s="17"/>
       <c r="AL38" s="18"/>
     </row>
-    <row r="39" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>43</v>
       </c>
@@ -2263,7 +2263,7 @@
       <c r="AK39" s="17"/>
       <c r="AL39" s="18"/>
     </row>
-    <row r="40" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
         <v>44</v>
       </c>
@@ -2307,7 +2307,7 @@
       <c r="AK40" s="28"/>
       <c r="AL40" s="30"/>
     </row>
-    <row r="41" spans="1:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="31"/>
       <c r="B41" s="32"/>
       <c r="C41" s="33"/>
@@ -2347,84 +2347,84 @@
       <c r="AK41" s="35"/>
       <c r="AL41" s="36"/>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A48" s="79" t="s">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A48" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="79"/>
-      <c r="C48" s="79"/>
-      <c r="D48" s="79"/>
-      <c r="E48" s="79"/>
-      <c r="F48" s="79"/>
-      <c r="G48" s="79"/>
-      <c r="H48" s="79"/>
-      <c r="I48" s="79"/>
-      <c r="J48" s="79"/>
-    </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A49" s="79"/>
-      <c r="B49" s="79"/>
-      <c r="C49" s="79"/>
-      <c r="D49" s="79"/>
-      <c r="E49" s="79"/>
-      <c r="F49" s="79"/>
-      <c r="G49" s="79"/>
-      <c r="H49" s="79"/>
-      <c r="I49" s="79"/>
-      <c r="J49" s="79"/>
-    </row>
-    <row r="50" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="51" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B48" s="95"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="95"/>
+      <c r="E48" s="95"/>
+      <c r="F48" s="95"/>
+      <c r="G48" s="95"/>
+      <c r="H48" s="95"/>
+      <c r="I48" s="95"/>
+      <c r="J48" s="95"/>
+    </row>
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A49" s="95"/>
+      <c r="B49" s="95"/>
+      <c r="C49" s="95"/>
+      <c r="D49" s="95"/>
+      <c r="E49" s="95"/>
+      <c r="F49" s="95"/>
+      <c r="G49" s="95"/>
+      <c r="H49" s="95"/>
+      <c r="I49" s="95"/>
+      <c r="J49" s="95"/>
+    </row>
+    <row r="50" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
-      <c r="D51" s="81" t="s">
+      <c r="D51" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="E51" s="82"/>
-      <c r="F51" s="82"/>
-      <c r="G51" s="82"/>
-      <c r="H51" s="82"/>
-      <c r="I51" s="82"/>
-      <c r="J51" s="83"/>
-      <c r="K51" s="92" t="s">
+      <c r="E51" s="86"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="86"/>
+      <c r="H51" s="86"/>
+      <c r="I51" s="86"/>
+      <c r="J51" s="87"/>
+      <c r="K51" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="L51" s="93"/>
-      <c r="M51" s="93"/>
-      <c r="N51" s="93"/>
-      <c r="O51" s="93"/>
-      <c r="P51" s="93"/>
-      <c r="Q51" s="93"/>
-      <c r="R51" s="81" t="s">
+      <c r="L51" s="89"/>
+      <c r="M51" s="89"/>
+      <c r="N51" s="89"/>
+      <c r="O51" s="89"/>
+      <c r="P51" s="89"/>
+      <c r="Q51" s="89"/>
+      <c r="R51" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="S51" s="82"/>
-      <c r="T51" s="82"/>
-      <c r="U51" s="82"/>
-      <c r="V51" s="82"/>
-      <c r="W51" s="82"/>
-      <c r="X51" s="83"/>
-      <c r="Y51" s="81" t="s">
+      <c r="S51" s="86"/>
+      <c r="T51" s="86"/>
+      <c r="U51" s="86"/>
+      <c r="V51" s="86"/>
+      <c r="W51" s="86"/>
+      <c r="X51" s="87"/>
+      <c r="Y51" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="Z51" s="84"/>
-      <c r="AA51" s="84"/>
-      <c r="AB51" s="84"/>
-      <c r="AC51" s="84"/>
-      <c r="AD51" s="84"/>
-      <c r="AE51" s="85"/>
-      <c r="AF51" s="81" t="s">
+      <c r="Z51" s="93"/>
+      <c r="AA51" s="93"/>
+      <c r="AB51" s="93"/>
+      <c r="AC51" s="93"/>
+      <c r="AD51" s="93"/>
+      <c r="AE51" s="94"/>
+      <c r="AF51" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="AG51" s="84"/>
-      <c r="AH51" s="84"/>
-      <c r="AI51" s="84"/>
-      <c r="AJ51" s="84"/>
-      <c r="AK51" s="84"/>
-      <c r="AL51" s="85"/>
-    </row>
-    <row r="52" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AG51" s="93"/>
+      <c r="AH51" s="93"/>
+      <c r="AI51" s="93"/>
+      <c r="AJ51" s="93"/>
+      <c r="AK51" s="93"/>
+      <c r="AL51" s="94"/>
+    </row>
+    <row r="52" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>6</v>
       </c>
@@ -2530,7 +2530,7 @@
       <c r="AK52" s="8"/>
       <c r="AL52" s="12"/>
     </row>
-    <row r="53" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>35</v>
       </c>
@@ -2574,7 +2574,7 @@
       <c r="AK53" s="17"/>
       <c r="AL53" s="18"/>
     </row>
-    <row r="54" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>47</v>
       </c>
@@ -2618,7 +2618,7 @@
       <c r="AK54" s="17"/>
       <c r="AL54" s="18"/>
     </row>
-    <row r="55" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>48</v>
       </c>
@@ -2662,7 +2662,7 @@
       <c r="AK55" s="17"/>
       <c r="AL55" s="18"/>
     </row>
-    <row r="56" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>49</v>
       </c>
@@ -2706,7 +2706,7 @@
       <c r="AK56" s="17"/>
       <c r="AL56" s="18"/>
     </row>
-    <row r="57" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>50</v>
       </c>
@@ -2752,7 +2752,7 @@
       <c r="AK57" s="17"/>
       <c r="AL57" s="18"/>
     </row>
-    <row r="58" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>51</v>
       </c>
@@ -2798,7 +2798,7 @@
       <c r="AK58" s="17"/>
       <c r="AL58" s="18"/>
     </row>
-    <row r="59" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>52</v>
       </c>
@@ -2842,7 +2842,7 @@
       <c r="AK59" s="17"/>
       <c r="AL59" s="18"/>
     </row>
-    <row r="60" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>53</v>
       </c>
@@ -2888,7 +2888,7 @@
       <c r="AK60" s="17"/>
       <c r="AL60" s="18"/>
     </row>
-    <row r="61" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="25" t="s">
         <v>55</v>
       </c>
@@ -2932,7 +2932,7 @@
       <c r="AK61" s="17"/>
       <c r="AL61" s="18"/>
     </row>
-    <row r="62" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="26" t="s">
         <v>56</v>
       </c>
@@ -2978,7 +2978,7 @@
       <c r="AK62" s="28"/>
       <c r="AL62" s="30"/>
     </row>
-    <row r="63" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
         <v>58</v>
       </c>
@@ -3024,7 +3024,7 @@
       <c r="AK63" s="17"/>
       <c r="AL63" s="18"/>
     </row>
-    <row r="64" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="59" t="s">
         <v>59</v>
       </c>
@@ -3070,7 +3070,7 @@
       <c r="AK64" s="65"/>
       <c r="AL64" s="66"/>
     </row>
-    <row r="65" spans="1:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="31"/>
       <c r="B65" s="32"/>
       <c r="C65" s="33"/>
@@ -3110,84 +3110,84 @@
       <c r="AK65" s="35"/>
       <c r="AL65" s="36"/>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A72" s="79" t="s">
+    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A72" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="B72" s="79"/>
-      <c r="C72" s="79"/>
-      <c r="D72" s="79"/>
-      <c r="E72" s="79"/>
-      <c r="F72" s="79"/>
-      <c r="G72" s="79"/>
-      <c r="H72" s="79"/>
-      <c r="I72" s="79"/>
-      <c r="J72" s="79"/>
-    </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A73" s="79"/>
-      <c r="B73" s="79"/>
-      <c r="C73" s="79"/>
-      <c r="D73" s="79"/>
-      <c r="E73" s="79"/>
-      <c r="F73" s="79"/>
-      <c r="G73" s="79"/>
-      <c r="H73" s="79"/>
-      <c r="I73" s="79"/>
-      <c r="J73" s="79"/>
-    </row>
-    <row r="74" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="75" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B72" s="95"/>
+      <c r="C72" s="95"/>
+      <c r="D72" s="95"/>
+      <c r="E72" s="95"/>
+      <c r="F72" s="95"/>
+      <c r="G72" s="95"/>
+      <c r="H72" s="95"/>
+      <c r="I72" s="95"/>
+      <c r="J72" s="95"/>
+    </row>
+    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A73" s="95"/>
+      <c r="B73" s="95"/>
+      <c r="C73" s="95"/>
+      <c r="D73" s="95"/>
+      <c r="E73" s="95"/>
+      <c r="F73" s="95"/>
+      <c r="G73" s="95"/>
+      <c r="H73" s="95"/>
+      <c r="I73" s="95"/>
+      <c r="J73" s="95"/>
+    </row>
+    <row r="74" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="4"/>
-      <c r="D75" s="82" t="s">
+      <c r="D75" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="E75" s="82"/>
-      <c r="F75" s="82"/>
-      <c r="G75" s="82"/>
-      <c r="H75" s="82"/>
-      <c r="I75" s="82"/>
-      <c r="J75" s="83"/>
-      <c r="K75" s="92" t="s">
+      <c r="E75" s="86"/>
+      <c r="F75" s="86"/>
+      <c r="G75" s="86"/>
+      <c r="H75" s="86"/>
+      <c r="I75" s="86"/>
+      <c r="J75" s="87"/>
+      <c r="K75" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="L75" s="93"/>
-      <c r="M75" s="93"/>
-      <c r="N75" s="93"/>
-      <c r="O75" s="93"/>
-      <c r="P75" s="93"/>
-      <c r="Q75" s="94"/>
-      <c r="R75" s="82" t="s">
+      <c r="L75" s="89"/>
+      <c r="M75" s="89"/>
+      <c r="N75" s="89"/>
+      <c r="O75" s="89"/>
+      <c r="P75" s="89"/>
+      <c r="Q75" s="103"/>
+      <c r="R75" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="S75" s="82"/>
-      <c r="T75" s="82"/>
-      <c r="U75" s="82"/>
-      <c r="V75" s="82"/>
-      <c r="W75" s="82"/>
-      <c r="X75" s="83"/>
-      <c r="Y75" s="81" t="s">
+      <c r="S75" s="86"/>
+      <c r="T75" s="86"/>
+      <c r="U75" s="86"/>
+      <c r="V75" s="86"/>
+      <c r="W75" s="86"/>
+      <c r="X75" s="87"/>
+      <c r="Y75" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="Z75" s="84"/>
-      <c r="AA75" s="84"/>
-      <c r="AB75" s="84"/>
-      <c r="AC75" s="84"/>
-      <c r="AD75" s="84"/>
-      <c r="AE75" s="85"/>
-      <c r="AF75" s="81" t="s">
+      <c r="Z75" s="93"/>
+      <c r="AA75" s="93"/>
+      <c r="AB75" s="93"/>
+      <c r="AC75" s="93"/>
+      <c r="AD75" s="93"/>
+      <c r="AE75" s="94"/>
+      <c r="AF75" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="AG75" s="84"/>
-      <c r="AH75" s="84"/>
-      <c r="AI75" s="84"/>
-      <c r="AJ75" s="84"/>
-      <c r="AK75" s="84"/>
-      <c r="AL75" s="85"/>
-    </row>
-    <row r="76" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AG75" s="93"/>
+      <c r="AH75" s="93"/>
+      <c r="AI75" s="93"/>
+      <c r="AJ75" s="93"/>
+      <c r="AK75" s="93"/>
+      <c r="AL75" s="94"/>
+    </row>
+    <row r="76" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>6</v>
       </c>
@@ -3295,7 +3295,7 @@
       <c r="AK76" s="8"/>
       <c r="AL76" s="12"/>
     </row>
-    <row r="77" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="59" t="s">
         <v>69</v>
       </c>
@@ -3341,7 +3341,7 @@
       <c r="AK77" s="17"/>
       <c r="AL77" s="18"/>
     </row>
-    <row r="78" spans="1:38" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:38" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>70</v>
       </c>
@@ -3382,7 +3382,7 @@
       <c r="AK78" s="17"/>
       <c r="AL78" s="18"/>
     </row>
-    <row r="79" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>65</v>
       </c>
@@ -3426,7 +3426,7 @@
       <c r="AK79" s="17"/>
       <c r="AL79" s="18"/>
     </row>
-    <row r="80" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
         <v>66</v>
       </c>
@@ -3472,7 +3472,7 @@
       <c r="AK80" s="17"/>
       <c r="AL80" s="18"/>
     </row>
-    <row r="81" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>68</v>
       </c>
@@ -3516,8 +3516,8 @@
       <c r="AK81" s="17"/>
       <c r="AL81" s="18"/>
     </row>
-    <row r="82" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="89" t="s">
+    <row r="82" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="99" t="s">
         <v>72</v>
       </c>
       <c r="B82" s="41"/>
@@ -3558,8 +3558,8 @@
       <c r="AK82" s="17"/>
       <c r="AL82" s="18"/>
     </row>
-    <row r="83" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="90"/>
+    <row r="83" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="100"/>
       <c r="B83" s="41"/>
       <c r="C83" s="77"/>
       <c r="D83" s="42"/>
@@ -3598,8 +3598,8 @@
       <c r="AK83" s="17"/>
       <c r="AL83" s="18"/>
     </row>
-    <row r="84" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="90"/>
+    <row r="84" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="100"/>
       <c r="B84" s="21"/>
       <c r="C84" s="15"/>
       <c r="D84" s="48"/>
@@ -3638,8 +3638,8 @@
       <c r="AK84" s="17"/>
       <c r="AL84" s="18"/>
     </row>
-    <row r="85" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="90"/>
+    <row r="85" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="100"/>
       <c r="B85" s="14"/>
       <c r="C85" s="15"/>
       <c r="D85" s="48"/>
@@ -3678,8 +3678,8 @@
       <c r="AK85" s="17"/>
       <c r="AL85" s="18"/>
     </row>
-    <row r="86" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="90"/>
+    <row r="86" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="100"/>
       <c r="B86" s="21"/>
       <c r="C86" s="15"/>
       <c r="D86" s="48"/>
@@ -3718,8 +3718,8 @@
       <c r="AK86" s="28"/>
       <c r="AL86" s="30"/>
     </row>
-    <row r="87" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="90"/>
+    <row r="87" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="100"/>
       <c r="B87" s="21"/>
       <c r="C87" s="15"/>
       <c r="D87" s="48"/>
@@ -3758,8 +3758,8 @@
       <c r="AK87" s="17"/>
       <c r="AL87" s="18"/>
     </row>
-    <row r="88" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="90"/>
+    <row r="88" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="100"/>
       <c r="B88" s="21"/>
       <c r="C88" s="15"/>
       <c r="D88" s="73"/>
@@ -3798,8 +3798,8 @@
       <c r="AK88" s="65"/>
       <c r="AL88" s="66"/>
     </row>
-    <row r="89" spans="1:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="91"/>
+    <row r="89" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="101"/>
       <c r="B89" s="74"/>
       <c r="C89" s="75"/>
       <c r="D89" s="78"/>
@@ -3838,84 +3838,84 @@
       <c r="AK89" s="35"/>
       <c r="AL89" s="36"/>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A96" s="79" t="s">
+    <row r="96" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A96" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="B96" s="79"/>
-      <c r="C96" s="79"/>
-      <c r="D96" s="79"/>
-      <c r="E96" s="79"/>
-      <c r="F96" s="79"/>
-      <c r="G96" s="79"/>
-      <c r="H96" s="79"/>
-      <c r="I96" s="79"/>
-      <c r="J96" s="79"/>
-    </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A97" s="79"/>
-      <c r="B97" s="79"/>
-      <c r="C97" s="79"/>
-      <c r="D97" s="79"/>
-      <c r="E97" s="79"/>
-      <c r="F97" s="79"/>
-      <c r="G97" s="79"/>
-      <c r="H97" s="79"/>
-      <c r="I97" s="79"/>
-      <c r="J97" s="79"/>
-    </row>
-    <row r="98" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="99" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B96" s="95"/>
+      <c r="C96" s="95"/>
+      <c r="D96" s="95"/>
+      <c r="E96" s="95"/>
+      <c r="F96" s="95"/>
+      <c r="G96" s="95"/>
+      <c r="H96" s="95"/>
+      <c r="I96" s="95"/>
+      <c r="J96" s="95"/>
+    </row>
+    <row r="97" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A97" s="95"/>
+      <c r="B97" s="95"/>
+      <c r="C97" s="95"/>
+      <c r="D97" s="95"/>
+      <c r="E97" s="95"/>
+      <c r="F97" s="95"/>
+      <c r="G97" s="95"/>
+      <c r="H97" s="95"/>
+      <c r="I97" s="95"/>
+      <c r="J97" s="95"/>
+    </row>
+    <row r="98" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="99" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="3"/>
       <c r="C99" s="4"/>
-      <c r="D99" s="81" t="s">
+      <c r="D99" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="E99" s="82"/>
-      <c r="F99" s="82"/>
-      <c r="G99" s="82"/>
-      <c r="H99" s="82"/>
-      <c r="I99" s="82"/>
-      <c r="J99" s="83"/>
-      <c r="K99" s="92" t="s">
+      <c r="E99" s="86"/>
+      <c r="F99" s="86"/>
+      <c r="G99" s="86"/>
+      <c r="H99" s="86"/>
+      <c r="I99" s="86"/>
+      <c r="J99" s="87"/>
+      <c r="K99" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="L99" s="93"/>
-      <c r="M99" s="93"/>
-      <c r="N99" s="93"/>
-      <c r="O99" s="93"/>
-      <c r="P99" s="93"/>
-      <c r="Q99" s="93"/>
-      <c r="R99" s="81" t="s">
+      <c r="L99" s="89"/>
+      <c r="M99" s="89"/>
+      <c r="N99" s="89"/>
+      <c r="O99" s="89"/>
+      <c r="P99" s="89"/>
+      <c r="Q99" s="89"/>
+      <c r="R99" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="S99" s="82"/>
-      <c r="T99" s="82"/>
-      <c r="U99" s="82"/>
-      <c r="V99" s="82"/>
-      <c r="W99" s="82"/>
-      <c r="X99" s="83"/>
-      <c r="Y99" s="81" t="s">
+      <c r="S99" s="86"/>
+      <c r="T99" s="86"/>
+      <c r="U99" s="86"/>
+      <c r="V99" s="86"/>
+      <c r="W99" s="86"/>
+      <c r="X99" s="87"/>
+      <c r="Y99" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="Z99" s="84"/>
-      <c r="AA99" s="84"/>
-      <c r="AB99" s="84"/>
-      <c r="AC99" s="84"/>
-      <c r="AD99" s="84"/>
-      <c r="AE99" s="85"/>
-      <c r="AF99" s="81" t="s">
+      <c r="Z99" s="93"/>
+      <c r="AA99" s="93"/>
+      <c r="AB99" s="93"/>
+      <c r="AC99" s="93"/>
+      <c r="AD99" s="93"/>
+      <c r="AE99" s="94"/>
+      <c r="AF99" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="AG99" s="84"/>
-      <c r="AH99" s="84"/>
-      <c r="AI99" s="84"/>
-      <c r="AJ99" s="84"/>
-      <c r="AK99" s="84"/>
-      <c r="AL99" s="85"/>
-    </row>
-    <row r="100" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AG99" s="93"/>
+      <c r="AH99" s="93"/>
+      <c r="AI99" s="93"/>
+      <c r="AJ99" s="93"/>
+      <c r="AK99" s="93"/>
+      <c r="AL99" s="94"/>
+    </row>
+    <row r="100" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>6</v>
       </c>
@@ -4021,7 +4021,7 @@
       <c r="AK100" s="8"/>
       <c r="AL100" s="12"/>
     </row>
-    <row r="101" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
         <v>71</v>
       </c>
@@ -4065,8 +4065,8 @@
       <c r="AK101" s="17"/>
       <c r="AL101" s="18"/>
     </row>
-    <row r="102" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="86" t="s">
+    <row r="102" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="96" t="s">
         <v>72</v>
       </c>
       <c r="B102" s="14"/>
@@ -4107,8 +4107,8 @@
       <c r="AK102" s="17"/>
       <c r="AL102" s="18"/>
     </row>
-    <row r="103" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A103" s="87"/>
+    <row r="103" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="97"/>
       <c r="B103" s="14"/>
       <c r="C103" s="15"/>
       <c r="D103" s="16"/>
@@ -4147,8 +4147,8 @@
       <c r="AK103" s="17"/>
       <c r="AL103" s="18"/>
     </row>
-    <row r="104" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="87"/>
+    <row r="104" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="97"/>
       <c r="B104" s="21"/>
       <c r="C104" s="15"/>
       <c r="D104" s="16"/>
@@ -4187,8 +4187,8 @@
       <c r="AK104" s="17"/>
       <c r="AL104" s="18"/>
     </row>
-    <row r="105" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="87"/>
+    <row r="105" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="97"/>
       <c r="B105" s="14"/>
       <c r="C105" s="22"/>
       <c r="D105" s="16"/>
@@ -4227,8 +4227,8 @@
       <c r="AK105" s="17"/>
       <c r="AL105" s="18"/>
     </row>
-    <row r="106" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="87"/>
+    <row r="106" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="97"/>
       <c r="B106" s="21"/>
       <c r="C106" s="22"/>
       <c r="D106" s="24"/>
@@ -4267,8 +4267,8 @@
       <c r="AK106" s="17"/>
       <c r="AL106" s="18"/>
     </row>
-    <row r="107" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="87"/>
+    <row r="107" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A107" s="97"/>
       <c r="B107" s="21"/>
       <c r="C107" s="22"/>
       <c r="D107" s="16"/>
@@ -4307,8 +4307,8 @@
       <c r="AK107" s="17"/>
       <c r="AL107" s="18"/>
     </row>
-    <row r="108" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="87"/>
+    <row r="108" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="97"/>
       <c r="B108" s="21"/>
       <c r="C108" s="15"/>
       <c r="D108" s="16"/>
@@ -4347,8 +4347,8 @@
       <c r="AK108" s="17"/>
       <c r="AL108" s="18"/>
     </row>
-    <row r="109" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" s="87"/>
+    <row r="109" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="97"/>
       <c r="B109" s="14"/>
       <c r="C109" s="15"/>
       <c r="D109" s="16"/>
@@ -4387,8 +4387,8 @@
       <c r="AK109" s="17"/>
       <c r="AL109" s="18"/>
     </row>
-    <row r="110" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A110" s="87"/>
+    <row r="110" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="97"/>
       <c r="B110" s="27"/>
       <c r="C110" s="15"/>
       <c r="D110" s="16"/>
@@ -4427,8 +4427,8 @@
       <c r="AK110" s="28"/>
       <c r="AL110" s="30"/>
     </row>
-    <row r="111" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="87"/>
+    <row r="111" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="97"/>
       <c r="B111" s="21"/>
       <c r="C111" s="15"/>
       <c r="D111" s="16"/>
@@ -4467,8 +4467,8 @@
       <c r="AK111" s="17"/>
       <c r="AL111" s="18"/>
     </row>
-    <row r="112" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="87"/>
+    <row r="112" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="97"/>
       <c r="B112" s="60"/>
       <c r="C112" s="61"/>
       <c r="D112" s="49"/>
@@ -4507,8 +4507,8 @@
       <c r="AK112" s="65"/>
       <c r="AL112" s="66"/>
     </row>
-    <row r="113" spans="1:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="88"/>
+    <row r="113" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="98"/>
       <c r="B113" s="32"/>
       <c r="C113" s="33"/>
       <c r="D113" s="34"/>
@@ -4547,84 +4547,84 @@
       <c r="AK113" s="35"/>
       <c r="AL113" s="36"/>
     </row>
-    <row r="120" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A120" s="79" t="s">
+    <row r="120" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A120" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="B120" s="79"/>
-      <c r="C120" s="79"/>
-      <c r="D120" s="79"/>
-      <c r="E120" s="79"/>
-      <c r="F120" s="79"/>
-      <c r="G120" s="79"/>
-      <c r="H120" s="79"/>
-      <c r="I120" s="79"/>
-      <c r="J120" s="79"/>
-    </row>
-    <row r="121" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A121" s="79"/>
-      <c r="B121" s="79"/>
-      <c r="C121" s="79"/>
-      <c r="D121" s="79"/>
-      <c r="E121" s="79"/>
-      <c r="F121" s="79"/>
-      <c r="G121" s="79"/>
-      <c r="H121" s="79"/>
-      <c r="I121" s="79"/>
-      <c r="J121" s="79"/>
-    </row>
-    <row r="122" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="123" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B120" s="95"/>
+      <c r="C120" s="95"/>
+      <c r="D120" s="95"/>
+      <c r="E120" s="95"/>
+      <c r="F120" s="95"/>
+      <c r="G120" s="95"/>
+      <c r="H120" s="95"/>
+      <c r="I120" s="95"/>
+      <c r="J120" s="95"/>
+    </row>
+    <row r="121" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A121" s="95"/>
+      <c r="B121" s="95"/>
+      <c r="C121" s="95"/>
+      <c r="D121" s="95"/>
+      <c r="E121" s="95"/>
+      <c r="F121" s="95"/>
+      <c r="G121" s="95"/>
+      <c r="H121" s="95"/>
+      <c r="I121" s="95"/>
+      <c r="J121" s="95"/>
+    </row>
+    <row r="122" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="3"/>
       <c r="C123" s="4"/>
-      <c r="D123" s="81" t="s">
+      <c r="D123" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="E123" s="82"/>
-      <c r="F123" s="82"/>
-      <c r="G123" s="82"/>
-      <c r="H123" s="82"/>
-      <c r="I123" s="82"/>
-      <c r="J123" s="83"/>
-      <c r="K123" s="92" t="s">
+      <c r="E123" s="86"/>
+      <c r="F123" s="86"/>
+      <c r="G123" s="86"/>
+      <c r="H123" s="86"/>
+      <c r="I123" s="86"/>
+      <c r="J123" s="87"/>
+      <c r="K123" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="L123" s="93"/>
-      <c r="M123" s="93"/>
-      <c r="N123" s="93"/>
-      <c r="O123" s="93"/>
-      <c r="P123" s="93"/>
-      <c r="Q123" s="93"/>
-      <c r="R123" s="81" t="s">
+      <c r="L123" s="89"/>
+      <c r="M123" s="89"/>
+      <c r="N123" s="89"/>
+      <c r="O123" s="89"/>
+      <c r="P123" s="89"/>
+      <c r="Q123" s="89"/>
+      <c r="R123" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="S123" s="82"/>
-      <c r="T123" s="82"/>
-      <c r="U123" s="82"/>
-      <c r="V123" s="82"/>
-      <c r="W123" s="82"/>
-      <c r="X123" s="83"/>
-      <c r="Y123" s="81" t="s">
+      <c r="S123" s="86"/>
+      <c r="T123" s="86"/>
+      <c r="U123" s="86"/>
+      <c r="V123" s="86"/>
+      <c r="W123" s="86"/>
+      <c r="X123" s="87"/>
+      <c r="Y123" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="Z123" s="84"/>
-      <c r="AA123" s="84"/>
-      <c r="AB123" s="84"/>
-      <c r="AC123" s="84"/>
-      <c r="AD123" s="84"/>
-      <c r="AE123" s="85"/>
-      <c r="AF123" s="81" t="s">
+      <c r="Z123" s="93"/>
+      <c r="AA123" s="93"/>
+      <c r="AB123" s="93"/>
+      <c r="AC123" s="93"/>
+      <c r="AD123" s="93"/>
+      <c r="AE123" s="94"/>
+      <c r="AF123" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="AG123" s="84"/>
-      <c r="AH123" s="84"/>
-      <c r="AI123" s="84"/>
-      <c r="AJ123" s="84"/>
-      <c r="AK123" s="84"/>
-      <c r="AL123" s="85"/>
-    </row>
-    <row r="124" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AG123" s="93"/>
+      <c r="AH123" s="93"/>
+      <c r="AI123" s="93"/>
+      <c r="AJ123" s="93"/>
+      <c r="AK123" s="93"/>
+      <c r="AL123" s="94"/>
+    </row>
+    <row r="124" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>6</v>
       </c>
@@ -4732,7 +4732,7 @@
       <c r="AK124" s="8"/>
       <c r="AL124" s="12"/>
     </row>
-    <row r="125" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
         <v>71</v>
       </c>
@@ -4776,8 +4776,8 @@
       <c r="AK125" s="17"/>
       <c r="AL125" s="18"/>
     </row>
-    <row r="126" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="86" t="s">
+    <row r="126" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A126" s="96" t="s">
         <v>72</v>
       </c>
       <c r="B126" s="14"/>
@@ -4818,8 +4818,8 @@
       <c r="AK126" s="17"/>
       <c r="AL126" s="18"/>
     </row>
-    <row r="127" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A127" s="87"/>
+    <row r="127" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A127" s="97"/>
       <c r="B127" s="14"/>
       <c r="C127" s="15"/>
       <c r="D127" s="16"/>
@@ -4858,8 +4858,8 @@
       <c r="AK127" s="17"/>
       <c r="AL127" s="18"/>
     </row>
-    <row r="128" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A128" s="87"/>
+    <row r="128" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A128" s="97"/>
       <c r="B128" s="21"/>
       <c r="C128" s="15"/>
       <c r="D128" s="16"/>
@@ -4898,8 +4898,8 @@
       <c r="AK128" s="17"/>
       <c r="AL128" s="18"/>
     </row>
-    <row r="129" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="87"/>
+    <row r="129" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A129" s="97"/>
       <c r="B129" s="14"/>
       <c r="C129" s="22"/>
       <c r="D129" s="16"/>
@@ -4938,8 +4938,8 @@
       <c r="AK129" s="17"/>
       <c r="AL129" s="18"/>
     </row>
-    <row r="130" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" s="87"/>
+    <row r="130" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A130" s="97"/>
       <c r="B130" s="21"/>
       <c r="C130" s="22"/>
       <c r="D130" s="24"/>
@@ -4978,8 +4978,8 @@
       <c r="AK130" s="17"/>
       <c r="AL130" s="18"/>
     </row>
-    <row r="131" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A131" s="87"/>
+    <row r="131" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A131" s="97"/>
       <c r="B131" s="21"/>
       <c r="C131" s="22"/>
       <c r="D131" s="16"/>
@@ -5018,8 +5018,8 @@
       <c r="AK131" s="17"/>
       <c r="AL131" s="18"/>
     </row>
-    <row r="132" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A132" s="87"/>
+    <row r="132" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A132" s="97"/>
       <c r="B132" s="21"/>
       <c r="C132" s="15"/>
       <c r="D132" s="16"/>
@@ -5058,8 +5058,8 @@
       <c r="AK132" s="17"/>
       <c r="AL132" s="18"/>
     </row>
-    <row r="133" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A133" s="87"/>
+    <row r="133" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A133" s="97"/>
       <c r="B133" s="14"/>
       <c r="C133" s="15"/>
       <c r="D133" s="16"/>
@@ -5098,8 +5098,8 @@
       <c r="AK133" s="17"/>
       <c r="AL133" s="18"/>
     </row>
-    <row r="134" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A134" s="87"/>
+    <row r="134" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A134" s="97"/>
       <c r="B134" s="27"/>
       <c r="C134" s="15"/>
       <c r="D134" s="16"/>
@@ -5138,8 +5138,8 @@
       <c r="AK134" s="28"/>
       <c r="AL134" s="30"/>
     </row>
-    <row r="135" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A135" s="87"/>
+    <row r="135" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A135" s="97"/>
       <c r="B135" s="21"/>
       <c r="C135" s="15"/>
       <c r="D135" s="16"/>
@@ -5178,8 +5178,8 @@
       <c r="AK135" s="17"/>
       <c r="AL135" s="18"/>
     </row>
-    <row r="136" spans="1:38" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A136" s="87"/>
+    <row r="136" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A136" s="97"/>
       <c r="B136" s="60"/>
       <c r="C136" s="61"/>
       <c r="D136" s="49"/>
@@ -5218,8 +5218,8 @@
       <c r="AK136" s="65"/>
       <c r="AL136" s="66"/>
     </row>
-    <row r="137" spans="1:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="88"/>
+    <row r="137" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="98"/>
       <c r="B137" s="32"/>
       <c r="C137" s="33"/>
       <c r="D137" s="34"/>
@@ -5260,35 +5260,6 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="K29:Q29"/>
-    <mergeCell ref="R29:X29"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="Y75:AE75"/>
-    <mergeCell ref="AF75:AL75"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="A48:J49"/>
-    <mergeCell ref="D51:J51"/>
-    <mergeCell ref="K51:Q51"/>
-    <mergeCell ref="R51:X51"/>
-    <mergeCell ref="A26:J27"/>
-    <mergeCell ref="Y29:AE29"/>
-    <mergeCell ref="AF29:AL29"/>
-    <mergeCell ref="A126:A137"/>
-    <mergeCell ref="A82:A89"/>
-    <mergeCell ref="A102:A113"/>
-    <mergeCell ref="A120:J121"/>
-    <mergeCell ref="D123:J123"/>
-    <mergeCell ref="A96:J97"/>
-    <mergeCell ref="D99:J99"/>
     <mergeCell ref="D3:K4"/>
     <mergeCell ref="C20:M21"/>
     <mergeCell ref="R123:X123"/>
@@ -5305,6 +5276,35 @@
     <mergeCell ref="D75:J75"/>
     <mergeCell ref="K75:Q75"/>
     <mergeCell ref="R75:X75"/>
+    <mergeCell ref="A126:A137"/>
+    <mergeCell ref="A82:A89"/>
+    <mergeCell ref="A102:A113"/>
+    <mergeCell ref="A120:J121"/>
+    <mergeCell ref="D123:J123"/>
+    <mergeCell ref="A96:J97"/>
+    <mergeCell ref="D99:J99"/>
+    <mergeCell ref="Y75:AE75"/>
+    <mergeCell ref="AF75:AL75"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="A48:J49"/>
+    <mergeCell ref="D51:J51"/>
+    <mergeCell ref="K51:Q51"/>
+    <mergeCell ref="R51:X51"/>
+    <mergeCell ref="A26:J27"/>
+    <mergeCell ref="Y29:AE29"/>
+    <mergeCell ref="AF29:AL29"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="K29:Q29"/>
+    <mergeCell ref="R29:X29"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>